<commit_message>
testing new system maybe 4.0...
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\P-Seminar\Git Rundgang\Rundgang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sync Drive\Schule\P-Seminar\Projekt\Rundgang so richtig rund!\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE85FC9D-9C59-41C1-8401-6695E32F4347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324E1C13-656D-4447-A7C7-04EE800B9061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6A5F55FC-30AE-4287-A9A7-03B76475C86E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A5F55FC-30AE-4287-A9A7-03B76475C86E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Todo:</t>
   </si>
@@ -185,6 +185,24 @@
   </si>
   <si>
     <t>? So oder anders?</t>
+  </si>
+  <si>
+    <t>Naviagation:</t>
+  </si>
+  <si>
+    <t>Treppen Icons auf der Karte - Maxi</t>
+  </si>
+  <si>
+    <t>Karte 1 Stock mit C Bau- Maxi</t>
+  </si>
+  <si>
+    <t>Alle Karten nochmal anpassen</t>
+  </si>
+  <si>
+    <t>Eastereggis</t>
+  </si>
+  <si>
+    <t>Tastenkombination….</t>
   </si>
 </sst>
 </file>
@@ -304,7 +322,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,9 +337,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -331,6 +346,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -648,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5112DD3-8621-44E7-A656-18F03BB2DF5F}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +697,7 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -720,12 +737,12 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
@@ -742,7 +759,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
@@ -753,12 +770,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -789,7 +806,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
@@ -797,7 +814,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="C18" t="s">
         <v>42</v>
       </c>
@@ -819,12 +838,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B23" t="s">
@@ -835,7 +854,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
@@ -843,12 +862,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B26" t="s">
@@ -870,18 +889,44 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>